<commit_message>
Added to informational tabs
</commit_message>
<xml_diff>
--- a/machine-creek/introduction-to-weka/predictSalesVolume.xlsx
+++ b/machine-creek/introduction-to-weka/predictSalesVolume.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/billy/Documents/HowTo/_WordPress/myContent/Weka KNN SVM/github/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/billy/repos/machine-creek/introduction-to-weka/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="40020" yWindow="960" windowWidth="26400" windowHeight="19340" tabRatio="385"/>
+    <workbookView xWindow="44980" yWindow="1800" windowWidth="26400" windowHeight="19340" tabRatio="385" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Existing Products" sheetId="8" r:id="rId1"/>
@@ -19,6 +19,8 @@
     <sheet name="DecisionTrees" sheetId="4" state="hidden" r:id="rId5"/>
     <sheet name="Potential New Prodcuts" sheetId="9" r:id="rId6"/>
     <sheet name="AutoWeka" sheetId="6" state="hidden" r:id="rId7"/>
+    <sheet name="Notes about characteristics" sheetId="10" r:id="rId8"/>
+    <sheet name="Warranty Scale" sheetId="11" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Existing Products'!$B$3:$V$40</definedName>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="245">
   <si>
     <t>k-Means Example</t>
   </si>
@@ -908,6 +910,48 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>Data Notes</t>
+  </si>
+  <si>
+    <t>5 star reviews, 4 star reviews, 3 star reviews, 2 star reviews, 1 star reviews</t>
+  </si>
+  <si>
+    <t>The value in the cell is the number of reviews level found on the web for the given product</t>
+  </si>
+  <si>
+    <t>The value in the cell is the number of positive service reviews  found on the web for the given product</t>
+  </si>
+  <si>
+    <t>The value in the cell is the number of negative service reviews  found on the web for the given product</t>
+  </si>
+  <si>
+    <t>Would consumer recommend product</t>
+  </si>
+  <si>
+    <t>The value in the cell is the percentage of customers who would recommend the product</t>
+  </si>
+  <si>
+    <t>The best sellers rank on Amazon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">See my comment in the example, I did not factor in this characteristic to the similarity analysis. </t>
+  </si>
+  <si>
+    <t>Coded Value</t>
+  </si>
+  <si>
+    <t>Rapid Replacement</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>This scale is applied to the Warranty Type column.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I have assumed that a limited warranty is better that no warranty, hardware warranty is better than a limited warranty, but worse than a Parts/Labor Warranty and so on. </t>
   </si>
 </sst>
 </file>
@@ -2615,7 +2659,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -2709,6 +2753,9 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="677" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="677" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2724,9 +2771,8 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="677" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="677" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="677" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1374">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -4493,7 +4539,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:X41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -7426,28 +7472,28 @@
       <c r="I10" s="5"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B12" s="57" t="s">
+      <c r="B12" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="57"/>
-      <c r="D12" s="57"/>
+      <c r="C12" s="58"/>
+      <c r="D12" s="58"/>
       <c r="E12" s="27"/>
-      <c r="F12" s="58" t="s">
+      <c r="F12" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="58"/>
-      <c r="H12" s="58"/>
+      <c r="G12" s="59"/>
+      <c r="H12" s="59"/>
       <c r="I12" s="26"/>
-      <c r="L12" s="57" t="s">
+      <c r="L12" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="M12" s="57"/>
-      <c r="N12" s="57"/>
-      <c r="P12" s="58" t="s">
+      <c r="M12" s="58"/>
+      <c r="N12" s="58"/>
+      <c r="P12" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="Q12" s="58"/>
-      <c r="R12" s="58"/>
+      <c r="Q12" s="59"/>
+      <c r="R12" s="59"/>
     </row>
     <row r="13" spans="1:18" ht="19" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
@@ -8993,10 +9039,10 @@
       <c r="J3" s="37"/>
       <c r="L3" s="39"/>
       <c r="M3" s="40"/>
-      <c r="N3" s="60" t="s">
+      <c r="N3" s="61" t="s">
         <v>110</v>
       </c>
-      <c r="O3" s="61"/>
+      <c r="O3" s="62"/>
       <c r="P3" s="41"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
@@ -9055,7 +9101,7 @@
       <c r="H5" s="37"/>
       <c r="I5" s="37"/>
       <c r="J5" s="37"/>
-      <c r="L5" s="59" t="s">
+      <c r="L5" s="60" t="s">
         <v>114</v>
       </c>
       <c r="M5" s="46" t="s">
@@ -9094,7 +9140,7 @@
       <c r="H6" s="37"/>
       <c r="I6" s="37"/>
       <c r="J6" s="37"/>
-      <c r="L6" s="59"/>
+      <c r="L6" s="60"/>
       <c r="M6" s="46" t="s">
         <v>114</v>
       </c>
@@ -9131,7 +9177,7 @@
       <c r="H7" s="37"/>
       <c r="I7" s="37"/>
       <c r="J7" s="37"/>
-      <c r="L7" s="59"/>
+      <c r="L7" s="60"/>
       <c r="M7" s="46" t="s">
         <v>115</v>
       </c>
@@ -9596,8 +9642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:S40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9722,7 +9768,7 @@
       <c r="R3" s="52">
         <v>0.25</v>
       </c>
-      <c r="S3" s="62" t="s">
+      <c r="S3" s="57" t="s">
         <v>230</v>
       </c>
     </row>
@@ -9778,7 +9824,7 @@
       <c r="R4" s="52">
         <v>0.2</v>
       </c>
-      <c r="S4" s="62" t="s">
+      <c r="S4" s="57" t="s">
         <v>230</v>
       </c>
     </row>
@@ -9834,7 +9880,7 @@
       <c r="R5" s="52">
         <v>0.1</v>
       </c>
-      <c r="S5" s="62" t="s">
+      <c r="S5" s="57" t="s">
         <v>230</v>
       </c>
     </row>
@@ -9890,7 +9936,7 @@
       <c r="R6" s="52">
         <v>0.15</v>
       </c>
-      <c r="S6" s="62" t="s">
+      <c r="S6" s="57" t="s">
         <v>230</v>
       </c>
     </row>
@@ -9946,7 +9992,7 @@
       <c r="R7" s="52">
         <v>0.23</v>
       </c>
-      <c r="S7" s="62" t="s">
+      <c r="S7" s="57" t="s">
         <v>230</v>
       </c>
     </row>
@@ -10002,7 +10048,7 @@
       <c r="R8" s="52">
         <v>0.08</v>
       </c>
-      <c r="S8" s="62" t="s">
+      <c r="S8" s="57" t="s">
         <v>230</v>
       </c>
     </row>
@@ -10058,7 +10104,7 @@
       <c r="R9" s="52">
         <v>0.09</v>
       </c>
-      <c r="S9" s="62" t="s">
+      <c r="S9" s="57" t="s">
         <v>230</v>
       </c>
     </row>
@@ -10114,7 +10160,7 @@
       <c r="R10" s="52">
         <v>0.11</v>
       </c>
-      <c r="S10" s="62" t="s">
+      <c r="S10" s="57" t="s">
         <v>230</v>
       </c>
     </row>
@@ -10170,7 +10216,7 @@
       <c r="R11" s="52">
         <v>0.09</v>
       </c>
-      <c r="S11" s="62" t="s">
+      <c r="S11" s="57" t="s">
         <v>230</v>
       </c>
     </row>
@@ -10226,7 +10272,7 @@
       <c r="R12" s="52">
         <v>0.1</v>
       </c>
-      <c r="S12" s="62" t="s">
+      <c r="S12" s="57" t="s">
         <v>230</v>
       </c>
     </row>
@@ -10282,7 +10328,7 @@
       <c r="R13" s="52">
         <v>0.2</v>
       </c>
-      <c r="S13" s="62" t="s">
+      <c r="S13" s="57" t="s">
         <v>230</v>
       </c>
     </row>
@@ -10338,7 +10384,7 @@
       <c r="R14" s="52">
         <v>0.11</v>
       </c>
-      <c r="S14" s="62" t="s">
+      <c r="S14" s="57" t="s">
         <v>230</v>
       </c>
     </row>
@@ -10394,7 +10440,7 @@
       <c r="R15" s="52">
         <v>0.12</v>
       </c>
-      <c r="S15" s="62" t="s">
+      <c r="S15" s="57" t="s">
         <v>230</v>
       </c>
     </row>
@@ -10450,7 +10496,7 @@
       <c r="R16" s="52">
         <v>0.15</v>
       </c>
-      <c r="S16" s="62" t="s">
+      <c r="S16" s="57" t="s">
         <v>230</v>
       </c>
     </row>
@@ -10506,7 +10552,7 @@
       <c r="R17" s="52">
         <v>0.11</v>
       </c>
-      <c r="S17" s="62" t="s">
+      <c r="S17" s="57" t="s">
         <v>230</v>
       </c>
     </row>
@@ -10562,7 +10608,7 @@
       <c r="R18" s="52">
         <v>0.09</v>
       </c>
-      <c r="S18" s="62" t="s">
+      <c r="S18" s="57" t="s">
         <v>230</v>
       </c>
     </row>
@@ -10618,8 +10664,64 @@
       <c r="R19" s="52">
         <v>0.05</v>
       </c>
-      <c r="S19" s="62" t="s">
+      <c r="S19" s="57" t="s">
         <v>230</v>
+      </c>
+    </row>
+    <row r="20" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B20" s="52">
+        <v>1</v>
+      </c>
+      <c r="C20" s="52">
+        <v>2</v>
+      </c>
+      <c r="D20" s="52">
+        <v>3</v>
+      </c>
+      <c r="E20" s="52">
+        <v>4</v>
+      </c>
+      <c r="F20" s="52">
+        <v>5</v>
+      </c>
+      <c r="G20" s="52">
+        <v>6</v>
+      </c>
+      <c r="H20" s="52">
+        <v>7</v>
+      </c>
+      <c r="I20" s="52">
+        <v>8</v>
+      </c>
+      <c r="J20" s="52">
+        <v>9</v>
+      </c>
+      <c r="K20" s="52">
+        <v>10</v>
+      </c>
+      <c r="L20" s="52">
+        <v>11</v>
+      </c>
+      <c r="M20" s="52">
+        <v>12</v>
+      </c>
+      <c r="N20" s="52">
+        <v>13</v>
+      </c>
+      <c r="O20" s="52">
+        <v>14</v>
+      </c>
+      <c r="P20" s="52">
+        <v>15</v>
+      </c>
+      <c r="Q20" s="52">
+        <v>16</v>
+      </c>
+      <c r="R20" s="52">
+        <v>17</v>
+      </c>
+      <c r="S20" s="52">
+        <v>18</v>
       </c>
     </row>
     <row r="40" spans="5:5" x14ac:dyDescent="0.2">
@@ -10822,4 +10924,166 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="45" style="52" customWidth="1"/>
+    <col min="2" max="16384" width="8.83203125" style="52"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="63" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="63" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="52" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="63" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="52" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="63" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="52" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="63" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="52" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" s="63" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="52" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="52" t="s">
+        <v>239</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.1640625" style="52" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" style="52" customWidth="1"/>
+    <col min="3" max="16384" width="11.5" style="52"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="63" t="s">
+        <v>162</v>
+      </c>
+      <c r="B1" s="63" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="64" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" s="64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="52" t="s">
+        <v>182</v>
+      </c>
+      <c r="B3" s="52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="52" t="s">
+        <v>221</v>
+      </c>
+      <c r="B4" s="52">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="52" t="s">
+        <v>185</v>
+      </c>
+      <c r="B5" s="52">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="52" t="s">
+        <v>241</v>
+      </c>
+      <c r="B6" s="52">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="52" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="52" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="52" t="s">
+        <v>244</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>